<commit_message>
child prog updated in fr books
</commit_message>
<xml_diff>
--- a/inputs/en/template_input.xlsx
+++ b/inputs/en/template_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\GitHub\Nutrition\inputs\en\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\modeling\Nutrition\inputs\en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB8B290-EF16-4630-92CF-D41EE9BBABC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E50E1CA-722B-4E93-9126-FFA943B20F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15225" yWindow="-18120" windowWidth="29040" windowHeight="17640" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="961" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -2925,9 +2925,6 @@
     <xf numFmtId="167" fontId="9" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
@@ -2935,6 +2932,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="725" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="728">
@@ -5110,7 +5110,7 @@
   </sheetPr>
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -6535,7 +6535,7 @@
   </sheetPr>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -12990,7 +12990,7 @@
       <c r="A2" s="29" t="s">
         <v>213</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="117" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="27" t="s">
@@ -13013,7 +13013,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="115"/>
+      <c r="B3" s="117"/>
       <c r="C3" s="27" t="s">
         <v>170</v>
       </c>
@@ -13035,7 +13035,7 @@
       <c r="J3" s="75"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="115"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="27" t="s">
         <v>169</v>
       </c>
@@ -13057,7 +13057,7 @@
       <c r="J4" s="75"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="117" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="27" t="s">
@@ -13081,7 +13081,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="115"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="27" t="s">
         <v>170</v>
       </c>
@@ -13102,7 +13102,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="115"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="27" t="s">
         <v>169</v>
       </c>
@@ -13123,7 +13123,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="115" t="s">
+      <c r="B8" s="117" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="27" t="s">
@@ -13146,7 +13146,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="115"/>
+      <c r="B9" s="117"/>
       <c r="C9" s="27" t="s">
         <v>170</v>
       </c>
@@ -13167,7 +13167,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="115"/>
+      <c r="B10" s="117"/>
       <c r="C10" s="27" t="s">
         <v>169</v>
       </c>
@@ -13188,7 +13188,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="115" t="s">
+      <c r="B11" s="117" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="27" t="s">
@@ -13211,7 +13211,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="115"/>
+      <c r="B12" s="117"/>
       <c r="C12" s="27" t="s">
         <v>170</v>
       </c>
@@ -13232,7 +13232,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="115"/>
+      <c r="B13" s="117"/>
       <c r="C13" s="27" t="s">
         <v>169</v>
       </c>
@@ -13253,7 +13253,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="115" t="s">
+      <c r="B14" s="117" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="27" t="s">
@@ -13276,7 +13276,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="115"/>
+      <c r="B15" s="117"/>
       <c r="C15" s="27" t="s">
         <v>170</v>
       </c>
@@ -13297,7 +13297,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="115"/>
+      <c r="B16" s="117"/>
       <c r="C16" s="27" t="s">
         <v>169</v>
       </c>
@@ -13351,7 +13351,7 @@
       <c r="A19" s="29" t="s">
         <v>214</v>
       </c>
-      <c r="B19" s="115" t="s">
+      <c r="B19" s="117" t="s">
         <v>32</v>
       </c>
       <c r="C19" s="27" t="s">
@@ -13374,7 +13374,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="115"/>
+      <c r="B20" s="117"/>
       <c r="C20" s="27" t="s">
         <v>170</v>
       </c>
@@ -13395,7 +13395,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="115"/>
+      <c r="B21" s="117"/>
       <c r="C21" s="27" t="s">
         <v>169</v>
       </c>
@@ -13416,7 +13416,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="115" t="s">
+      <c r="B22" s="117" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="27" t="s">
@@ -13439,7 +13439,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="115"/>
+      <c r="B23" s="117"/>
       <c r="C23" s="27" t="s">
         <v>170</v>
       </c>
@@ -13460,7 +13460,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="115"/>
+      <c r="B24" s="117"/>
       <c r="C24" s="27" t="s">
         <v>169</v>
       </c>
@@ -13481,7 +13481,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="115" t="s">
+      <c r="B25" s="117" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="27" t="s">
@@ -13504,7 +13504,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="115"/>
+      <c r="B26" s="117"/>
       <c r="C26" s="27" t="s">
         <v>170</v>
       </c>
@@ -13525,7 +13525,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="115"/>
+      <c r="B27" s="117"/>
       <c r="C27" s="27" t="s">
         <v>169</v>
       </c>
@@ -13546,7 +13546,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="115" t="s">
+      <c r="B28" s="117" t="s">
         <v>3</v>
       </c>
       <c r="C28" s="27" t="s">
@@ -13569,7 +13569,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="115"/>
+      <c r="B29" s="117"/>
       <c r="C29" s="27" t="s">
         <v>170</v>
       </c>
@@ -13590,7 +13590,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="115"/>
+      <c r="B30" s="117"/>
       <c r="C30" s="27" t="s">
         <v>169</v>
       </c>
@@ -13611,7 +13611,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="115" t="s">
+      <c r="B31" s="117" t="s">
         <v>4</v>
       </c>
       <c r="C31" s="27" t="s">
@@ -13634,7 +13634,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="115"/>
+      <c r="B32" s="117"/>
       <c r="C32" s="27" t="s">
         <v>170</v>
       </c>
@@ -13655,7 +13655,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="115"/>
+      <c r="B33" s="117"/>
       <c r="C33" s="27" t="s">
         <v>169</v>
       </c>
@@ -13709,7 +13709,7 @@
       <c r="A36" s="77" t="s">
         <v>215</v>
       </c>
-      <c r="B36" s="115" t="s">
+      <c r="B36" s="117" t="s">
         <v>32</v>
       </c>
       <c r="C36" s="27" t="s">
@@ -13732,7 +13732,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="115"/>
+      <c r="B37" s="117"/>
       <c r="C37" s="27" t="s">
         <v>170</v>
       </c>
@@ -13753,7 +13753,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="115"/>
+      <c r="B38" s="117"/>
       <c r="C38" s="27" t="s">
         <v>169</v>
       </c>
@@ -13774,7 +13774,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="115" t="s">
+      <c r="B39" s="117" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="27" t="s">
@@ -13797,7 +13797,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="115"/>
+      <c r="B40" s="117"/>
       <c r="C40" s="27" t="s">
         <v>170</v>
       </c>
@@ -13818,7 +13818,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="115"/>
+      <c r="B41" s="117"/>
       <c r="C41" s="27" t="s">
         <v>169</v>
       </c>
@@ -13839,7 +13839,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="115" t="s">
+      <c r="B42" s="117" t="s">
         <v>2</v>
       </c>
       <c r="C42" s="27" t="s">
@@ -13862,7 +13862,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="115"/>
+      <c r="B43" s="117"/>
       <c r="C43" s="27" t="s">
         <v>170</v>
       </c>
@@ -13883,7 +13883,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="115"/>
+      <c r="B44" s="117"/>
       <c r="C44" s="27" t="s">
         <v>169</v>
       </c>
@@ -13904,7 +13904,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="115" t="s">
+      <c r="B45" s="117" t="s">
         <v>3</v>
       </c>
       <c r="C45" s="27" t="s">
@@ -13927,7 +13927,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="115"/>
+      <c r="B46" s="117"/>
       <c r="C46" s="27" t="s">
         <v>170</v>
       </c>
@@ -13948,7 +13948,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="115"/>
+      <c r="B47" s="117"/>
       <c r="C47" s="27" t="s">
         <v>169</v>
       </c>
@@ -13969,7 +13969,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="115" t="s">
+      <c r="B48" s="117" t="s">
         <v>4</v>
       </c>
       <c r="C48" s="27" t="s">
@@ -13992,7 +13992,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="115"/>
+      <c r="B49" s="117"/>
       <c r="C49" s="27" t="s">
         <v>170</v>
       </c>
@@ -14013,7 +14013,7 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="115"/>
+      <c r="B50" s="117"/>
       <c r="C50" s="27" t="s">
         <v>169</v>
       </c>
@@ -14098,7 +14098,7 @@
       <c r="A55" s="29" t="s">
         <v>311</v>
       </c>
-      <c r="B55" s="115" t="s">
+      <c r="B55" s="117" t="s">
         <v>32</v>
       </c>
       <c r="C55" s="27" t="s">
@@ -14126,7 +14126,7 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="115"/>
+      <c r="B56" s="117"/>
       <c r="C56" s="27" t="s">
         <v>170</v>
       </c>
@@ -14152,7 +14152,7 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="115"/>
+      <c r="B57" s="117"/>
       <c r="C57" s="27" t="s">
         <v>169</v>
       </c>
@@ -14178,7 +14178,7 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B58" s="115" t="s">
+      <c r="B58" s="117" t="s">
         <v>1</v>
       </c>
       <c r="C58" s="27" t="s">
@@ -14206,7 +14206,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="115"/>
+      <c r="B59" s="117"/>
       <c r="C59" s="27" t="s">
         <v>170</v>
       </c>
@@ -14232,7 +14232,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="115"/>
+      <c r="B60" s="117"/>
       <c r="C60" s="27" t="s">
         <v>169</v>
       </c>
@@ -14258,7 +14258,7 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="115" t="s">
+      <c r="B61" s="117" t="s">
         <v>2</v>
       </c>
       <c r="C61" s="27" t="s">
@@ -14286,7 +14286,7 @@
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="115"/>
+      <c r="B62" s="117"/>
       <c r="C62" s="27" t="s">
         <v>170</v>
       </c>
@@ -14312,7 +14312,7 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="115"/>
+      <c r="B63" s="117"/>
       <c r="C63" s="27" t="s">
         <v>169</v>
       </c>
@@ -14338,7 +14338,7 @@
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B64" s="115" t="s">
+      <c r="B64" s="117" t="s">
         <v>3</v>
       </c>
       <c r="C64" s="27" t="s">
@@ -14366,7 +14366,7 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B65" s="115"/>
+      <c r="B65" s="117"/>
       <c r="C65" s="27" t="s">
         <v>170</v>
       </c>
@@ -14392,7 +14392,7 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="115"/>
+      <c r="B66" s="117"/>
       <c r="C66" s="27" t="s">
         <v>169</v>
       </c>
@@ -14418,7 +14418,7 @@
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="115" t="s">
+      <c r="B67" s="117" t="s">
         <v>4</v>
       </c>
       <c r="C67" s="27" t="s">
@@ -14446,7 +14446,7 @@
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="115"/>
+      <c r="B68" s="117"/>
       <c r="C68" s="27" t="s">
         <v>170</v>
       </c>
@@ -14472,7 +14472,7 @@
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="115"/>
+      <c r="B69" s="117"/>
       <c r="C69" s="27" t="s">
         <v>169</v>
       </c>
@@ -14536,7 +14536,7 @@
       <c r="A72" s="29" t="s">
         <v>312</v>
       </c>
-      <c r="B72" s="115" t="s">
+      <c r="B72" s="117" t="s">
         <v>32</v>
       </c>
       <c r="C72" s="27" t="s">
@@ -14564,7 +14564,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B73" s="115"/>
+      <c r="B73" s="117"/>
       <c r="C73" s="27" t="s">
         <v>170</v>
       </c>
@@ -14590,7 +14590,7 @@
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B74" s="115"/>
+      <c r="B74" s="117"/>
       <c r="C74" s="27" t="s">
         <v>169</v>
       </c>
@@ -14616,7 +14616,7 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="115" t="s">
+      <c r="B75" s="117" t="s">
         <v>1</v>
       </c>
       <c r="C75" s="27" t="s">
@@ -14644,7 +14644,7 @@
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B76" s="115"/>
+      <c r="B76" s="117"/>
       <c r="C76" s="27" t="s">
         <v>170</v>
       </c>
@@ -14670,7 +14670,7 @@
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B77" s="115"/>
+      <c r="B77" s="117"/>
       <c r="C77" s="27" t="s">
         <v>169</v>
       </c>
@@ -14696,7 +14696,7 @@
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B78" s="115" t="s">
+      <c r="B78" s="117" t="s">
         <v>2</v>
       </c>
       <c r="C78" s="27" t="s">
@@ -14724,7 +14724,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B79" s="115"/>
+      <c r="B79" s="117"/>
       <c r="C79" s="27" t="s">
         <v>170</v>
       </c>
@@ -14750,7 +14750,7 @@
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B80" s="115"/>
+      <c r="B80" s="117"/>
       <c r="C80" s="27" t="s">
         <v>169</v>
       </c>
@@ -14776,7 +14776,7 @@
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B81" s="115" t="s">
+      <c r="B81" s="117" t="s">
         <v>3</v>
       </c>
       <c r="C81" s="27" t="s">
@@ -14804,7 +14804,7 @@
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B82" s="115"/>
+      <c r="B82" s="117"/>
       <c r="C82" s="27" t="s">
         <v>170</v>
       </c>
@@ -14830,7 +14830,7 @@
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="115"/>
+      <c r="B83" s="117"/>
       <c r="C83" s="27" t="s">
         <v>169</v>
       </c>
@@ -14856,7 +14856,7 @@
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B84" s="115" t="s">
+      <c r="B84" s="117" t="s">
         <v>4</v>
       </c>
       <c r="C84" s="27" t="s">
@@ -14884,7 +14884,7 @@
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B85" s="115"/>
+      <c r="B85" s="117"/>
       <c r="C85" s="27" t="s">
         <v>170</v>
       </c>
@@ -14910,7 +14910,7 @@
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B86" s="115"/>
+      <c r="B86" s="117"/>
       <c r="C86" s="27" t="s">
         <v>169</v>
       </c>
@@ -14974,7 +14974,7 @@
       <c r="A89" s="77" t="s">
         <v>313</v>
       </c>
-      <c r="B89" s="115" t="s">
+      <c r="B89" s="117" t="s">
         <v>32</v>
       </c>
       <c r="C89" s="27" t="s">
@@ -15002,7 +15002,7 @@
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B90" s="115"/>
+      <c r="B90" s="117"/>
       <c r="C90" s="27" t="s">
         <v>170</v>
       </c>
@@ -15028,7 +15028,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B91" s="115"/>
+      <c r="B91" s="117"/>
       <c r="C91" s="27" t="s">
         <v>169</v>
       </c>
@@ -15054,7 +15054,7 @@
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B92" s="115" t="s">
+      <c r="B92" s="117" t="s">
         <v>1</v>
       </c>
       <c r="C92" s="27" t="s">
@@ -15082,7 +15082,7 @@
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B93" s="115"/>
+      <c r="B93" s="117"/>
       <c r="C93" s="27" t="s">
         <v>170</v>
       </c>
@@ -15108,7 +15108,7 @@
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B94" s="115"/>
+      <c r="B94" s="117"/>
       <c r="C94" s="27" t="s">
         <v>169</v>
       </c>
@@ -15134,7 +15134,7 @@
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="115" t="s">
+      <c r="B95" s="117" t="s">
         <v>2</v>
       </c>
       <c r="C95" s="27" t="s">
@@ -15162,7 +15162,7 @@
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B96" s="115"/>
+      <c r="B96" s="117"/>
       <c r="C96" s="27" t="s">
         <v>170</v>
       </c>
@@ -15188,7 +15188,7 @@
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B97" s="115"/>
+      <c r="B97" s="117"/>
       <c r="C97" s="27" t="s">
         <v>169</v>
       </c>
@@ -15214,7 +15214,7 @@
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B98" s="115" t="s">
+      <c r="B98" s="117" t="s">
         <v>3</v>
       </c>
       <c r="C98" s="27" t="s">
@@ -15242,7 +15242,7 @@
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B99" s="115"/>
+      <c r="B99" s="117"/>
       <c r="C99" s="27" t="s">
         <v>170</v>
       </c>
@@ -15268,7 +15268,7 @@
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B100" s="115"/>
+      <c r="B100" s="117"/>
       <c r="C100" s="27" t="s">
         <v>169</v>
       </c>
@@ -15294,7 +15294,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B101" s="115" t="s">
+      <c r="B101" s="117" t="s">
         <v>4</v>
       </c>
       <c r="C101" s="27" t="s">
@@ -15322,7 +15322,7 @@
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B102" s="115"/>
+      <c r="B102" s="117"/>
       <c r="C102" s="27" t="s">
         <v>170</v>
       </c>
@@ -15348,7 +15348,7 @@
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B103" s="115"/>
+      <c r="B103" s="117"/>
       <c r="C103" s="27" t="s">
         <v>169</v>
       </c>
@@ -15443,7 +15443,7 @@
       <c r="A108" s="29" t="s">
         <v>314</v>
       </c>
-      <c r="B108" s="115" t="s">
+      <c r="B108" s="117" t="s">
         <v>32</v>
       </c>
       <c r="C108" s="27" t="s">
@@ -15471,7 +15471,7 @@
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B109" s="115"/>
+      <c r="B109" s="117"/>
       <c r="C109" s="27" t="s">
         <v>170</v>
       </c>
@@ -15497,7 +15497,7 @@
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B110" s="115"/>
+      <c r="B110" s="117"/>
       <c r="C110" s="27" t="s">
         <v>169</v>
       </c>
@@ -15523,7 +15523,7 @@
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B111" s="115" t="s">
+      <c r="B111" s="117" t="s">
         <v>1</v>
       </c>
       <c r="C111" s="27" t="s">
@@ -15551,7 +15551,7 @@
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B112" s="115"/>
+      <c r="B112" s="117"/>
       <c r="C112" s="27" t="s">
         <v>170</v>
       </c>
@@ -15577,7 +15577,7 @@
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B113" s="115"/>
+      <c r="B113" s="117"/>
       <c r="C113" s="27" t="s">
         <v>169</v>
       </c>
@@ -15603,7 +15603,7 @@
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B114" s="115" t="s">
+      <c r="B114" s="117" t="s">
         <v>2</v>
       </c>
       <c r="C114" s="27" t="s">
@@ -15631,7 +15631,7 @@
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B115" s="115"/>
+      <c r="B115" s="117"/>
       <c r="C115" s="27" t="s">
         <v>170</v>
       </c>
@@ -15657,7 +15657,7 @@
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B116" s="115"/>
+      <c r="B116" s="117"/>
       <c r="C116" s="27" t="s">
         <v>169</v>
       </c>
@@ -15683,7 +15683,7 @@
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B117" s="115" t="s">
+      <c r="B117" s="117" t="s">
         <v>3</v>
       </c>
       <c r="C117" s="27" t="s">
@@ -15711,7 +15711,7 @@
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B118" s="115"/>
+      <c r="B118" s="117"/>
       <c r="C118" s="27" t="s">
         <v>170</v>
       </c>
@@ -15737,7 +15737,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B119" s="115"/>
+      <c r="B119" s="117"/>
       <c r="C119" s="27" t="s">
         <v>169</v>
       </c>
@@ -15763,7 +15763,7 @@
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B120" s="115" t="s">
+      <c r="B120" s="117" t="s">
         <v>4</v>
       </c>
       <c r="C120" s="27" t="s">
@@ -15791,7 +15791,7 @@
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B121" s="115"/>
+      <c r="B121" s="117"/>
       <c r="C121" s="27" t="s">
         <v>170</v>
       </c>
@@ -15817,7 +15817,7 @@
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B122" s="115"/>
+      <c r="B122" s="117"/>
       <c r="C122" s="27" t="s">
         <v>169</v>
       </c>
@@ -15881,7 +15881,7 @@
       <c r="A125" s="29" t="s">
         <v>315</v>
       </c>
-      <c r="B125" s="115" t="s">
+      <c r="B125" s="117" t="s">
         <v>32</v>
       </c>
       <c r="C125" s="27" t="s">
@@ -15909,7 +15909,7 @@
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B126" s="115"/>
+      <c r="B126" s="117"/>
       <c r="C126" s="27" t="s">
         <v>170</v>
       </c>
@@ -15935,7 +15935,7 @@
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B127" s="115"/>
+      <c r="B127" s="117"/>
       <c r="C127" s="27" t="s">
         <v>169</v>
       </c>
@@ -15961,7 +15961,7 @@
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B128" s="115" t="s">
+      <c r="B128" s="117" t="s">
         <v>1</v>
       </c>
       <c r="C128" s="27" t="s">
@@ -15989,7 +15989,7 @@
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B129" s="115"/>
+      <c r="B129" s="117"/>
       <c r="C129" s="27" t="s">
         <v>170</v>
       </c>
@@ -16015,7 +16015,7 @@
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B130" s="115"/>
+      <c r="B130" s="117"/>
       <c r="C130" s="27" t="s">
         <v>169</v>
       </c>
@@ -16041,7 +16041,7 @@
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B131" s="115" t="s">
+      <c r="B131" s="117" t="s">
         <v>2</v>
       </c>
       <c r="C131" s="27" t="s">
@@ -16069,7 +16069,7 @@
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B132" s="115"/>
+      <c r="B132" s="117"/>
       <c r="C132" s="27" t="s">
         <v>170</v>
       </c>
@@ -16095,7 +16095,7 @@
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B133" s="115"/>
+      <c r="B133" s="117"/>
       <c r="C133" s="27" t="s">
         <v>169</v>
       </c>
@@ -16121,7 +16121,7 @@
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B134" s="115" t="s">
+      <c r="B134" s="117" t="s">
         <v>3</v>
       </c>
       <c r="C134" s="27" t="s">
@@ -16149,7 +16149,7 @@
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B135" s="115"/>
+      <c r="B135" s="117"/>
       <c r="C135" s="27" t="s">
         <v>170</v>
       </c>
@@ -16175,7 +16175,7 @@
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B136" s="115"/>
+      <c r="B136" s="117"/>
       <c r="C136" s="27" t="s">
         <v>169</v>
       </c>
@@ -16201,7 +16201,7 @@
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B137" s="115" t="s">
+      <c r="B137" s="117" t="s">
         <v>4</v>
       </c>
       <c r="C137" s="27" t="s">
@@ -16229,7 +16229,7 @@
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B138" s="115"/>
+      <c r="B138" s="117"/>
       <c r="C138" s="27" t="s">
         <v>170</v>
       </c>
@@ -16255,7 +16255,7 @@
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B139" s="115"/>
+      <c r="B139" s="117"/>
       <c r="C139" s="27" t="s">
         <v>169</v>
       </c>
@@ -16319,7 +16319,7 @@
       <c r="A142" s="77" t="s">
         <v>316</v>
       </c>
-      <c r="B142" s="115" t="s">
+      <c r="B142" s="117" t="s">
         <v>32</v>
       </c>
       <c r="C142" s="27" t="s">
@@ -16347,7 +16347,7 @@
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B143" s="115"/>
+      <c r="B143" s="117"/>
       <c r="C143" s="27" t="s">
         <v>170</v>
       </c>
@@ -16373,7 +16373,7 @@
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B144" s="115"/>
+      <c r="B144" s="117"/>
       <c r="C144" s="27" t="s">
         <v>169</v>
       </c>
@@ -16399,7 +16399,7 @@
       </c>
     </row>
     <row r="145" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B145" s="115" t="s">
+      <c r="B145" s="117" t="s">
         <v>1</v>
       </c>
       <c r="C145" s="27" t="s">
@@ -16427,7 +16427,7 @@
       </c>
     </row>
     <row r="146" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B146" s="115"/>
+      <c r="B146" s="117"/>
       <c r="C146" s="27" t="s">
         <v>170</v>
       </c>
@@ -16453,7 +16453,7 @@
       </c>
     </row>
     <row r="147" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B147" s="115"/>
+      <c r="B147" s="117"/>
       <c r="C147" s="27" t="s">
         <v>169</v>
       </c>
@@ -16479,7 +16479,7 @@
       </c>
     </row>
     <row r="148" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B148" s="115" t="s">
+      <c r="B148" s="117" t="s">
         <v>2</v>
       </c>
       <c r="C148" s="27" t="s">
@@ -16507,7 +16507,7 @@
       </c>
     </row>
     <row r="149" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B149" s="115"/>
+      <c r="B149" s="117"/>
       <c r="C149" s="27" t="s">
         <v>170</v>
       </c>
@@ -16533,7 +16533,7 @@
       </c>
     </row>
     <row r="150" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B150" s="115"/>
+      <c r="B150" s="117"/>
       <c r="C150" s="27" t="s">
         <v>169</v>
       </c>
@@ -16559,7 +16559,7 @@
       </c>
     </row>
     <row r="151" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B151" s="115" t="s">
+      <c r="B151" s="117" t="s">
         <v>3</v>
       </c>
       <c r="C151" s="27" t="s">
@@ -16587,7 +16587,7 @@
       </c>
     </row>
     <row r="152" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B152" s="115"/>
+      <c r="B152" s="117"/>
       <c r="C152" s="27" t="s">
         <v>170</v>
       </c>
@@ -16613,7 +16613,7 @@
       </c>
     </row>
     <row r="153" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B153" s="115"/>
+      <c r="B153" s="117"/>
       <c r="C153" s="27" t="s">
         <v>169</v>
       </c>
@@ -16639,7 +16639,7 @@
       </c>
     </row>
     <row r="154" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B154" s="115" t="s">
+      <c r="B154" s="117" t="s">
         <v>4</v>
       </c>
       <c r="C154" s="27" t="s">
@@ -16667,7 +16667,7 @@
       </c>
     </row>
     <row r="155" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B155" s="115"/>
+      <c r="B155" s="117"/>
       <c r="C155" s="27" t="s">
         <v>170</v>
       </c>
@@ -16693,7 +16693,7 @@
       </c>
     </row>
     <row r="156" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B156" s="115"/>
+      <c r="B156" s="117"/>
       <c r="C156" s="27" t="s">
         <v>169</v>
       </c>
@@ -16749,12 +16749,36 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="tLFUmDyoH82P3agTzdNhIl/nrPXW114misPcwvY90QMxHUTQPj6nXWoXArIchS0+Y1PkNffvDNQ/0vLhBaHAnA==" saltValue="GmZrDncYr09T1PgEJ065qQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="45">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B145:B147"/>
+    <mergeCell ref="B148:B150"/>
+    <mergeCell ref="B151:B153"/>
+    <mergeCell ref="B154:B156"/>
+    <mergeCell ref="B128:B130"/>
+    <mergeCell ref="B131:B133"/>
+    <mergeCell ref="B134:B136"/>
+    <mergeCell ref="B137:B139"/>
+    <mergeCell ref="B142:B144"/>
+    <mergeCell ref="B111:B113"/>
+    <mergeCell ref="B114:B116"/>
+    <mergeCell ref="B117:B119"/>
+    <mergeCell ref="B120:B122"/>
+    <mergeCell ref="B125:B127"/>
+    <mergeCell ref="B108:B110"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="B101:B103"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B67:B69"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -16764,36 +16788,12 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="B108:B110"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="B92:B94"/>
-    <mergeCell ref="B95:B97"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="B101:B103"/>
-    <mergeCell ref="B111:B113"/>
-    <mergeCell ref="B114:B116"/>
-    <mergeCell ref="B117:B119"/>
-    <mergeCell ref="B120:B122"/>
-    <mergeCell ref="B125:B127"/>
-    <mergeCell ref="B145:B147"/>
-    <mergeCell ref="B148:B150"/>
-    <mergeCell ref="B151:B153"/>
-    <mergeCell ref="B154:B156"/>
-    <mergeCell ref="B128:B130"/>
-    <mergeCell ref="B131:B133"/>
-    <mergeCell ref="B134:B136"/>
-    <mergeCell ref="B137:B139"/>
-    <mergeCell ref="B142:B144"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -31311,8 +31311,8 @@
   </sheetPr>
   <dimension ref="A1:H163"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D112" sqref="D112"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -31371,13 +31371,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="104">
-        <v>0.33500000000000002</v>
+        <v>0.39473684210526322</v>
       </c>
       <c r="G2" s="104">
-        <v>0.33500000000000002</v>
+        <v>0.39473684210526322</v>
       </c>
       <c r="H2" s="104">
-        <v>0.33500000000000002</v>
+        <v>0.39473684210526322</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -31391,13 +31391,13 @@
         <v>0</v>
       </c>
       <c r="F3" s="104">
-        <v>0.53134328358208949</v>
+        <v>0.30769230769230765</v>
       </c>
       <c r="G3" s="104">
-        <v>0.53134328358208949</v>
+        <v>0.30769230769230765</v>
       </c>
       <c r="H3" s="104">
-        <v>0.53134328358208949</v>
+        <v>0.30769230769230765</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -31724,7 +31724,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="104">
-        <v>0.33500000000000002</v>
+        <v>0.7</v>
       </c>
       <c r="G18" s="104">
         <v>0.62</v>
@@ -31767,7 +31767,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="104">
-        <v>0.33500000000000002</v>
+        <v>0.84</v>
       </c>
       <c r="G20" s="104">
         <v>0.62</v>
@@ -31787,13 +31787,13 @@
         <v>261</v>
       </c>
       <c r="D21" s="104">
-        <v>0.7</v>
+        <v>0.28260869565217389</v>
       </c>
       <c r="E21" s="104">
         <v>0</v>
       </c>
       <c r="F21" s="104">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G21" s="104">
         <v>0</v>
@@ -31813,7 +31813,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="104">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G22" s="104">
         <v>0</v>
@@ -31833,13 +31833,13 @@
         <v>261</v>
       </c>
       <c r="D23" s="104">
-        <v>0.7</v>
+        <v>0.28260869565217389</v>
       </c>
       <c r="E23" s="104">
         <v>0</v>
       </c>
       <c r="F23" s="104">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G23" s="104">
         <v>0</v>
@@ -31859,7 +31859,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="104">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G24" s="104">
         <v>0</v>
@@ -31879,13 +31879,13 @@
         <v>261</v>
       </c>
       <c r="D25" s="104">
-        <v>0.7</v>
+        <v>0.28260869565217389</v>
       </c>
       <c r="E25" s="104">
         <v>0</v>
       </c>
       <c r="F25" s="104">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G25" s="104">
         <v>0</v>
@@ -31905,7 +31905,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="104">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G26" s="104">
         <v>0</v>
@@ -31931,7 +31931,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="104">
-        <v>0.33500000000000002</v>
+        <v>1</v>
       </c>
       <c r="G27" s="104">
         <v>1</v>
@@ -31951,7 +31951,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="104">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G28" s="104">
         <v>0</v>
@@ -31971,7 +31971,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="104">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G29" s="104">
         <v>0</v>
@@ -31997,7 +31997,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="104">
-        <v>0.33500000000000002</v>
+        <v>1</v>
       </c>
       <c r="G30" s="104">
         <v>1</v>
@@ -32017,7 +32017,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="104">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G31" s="104">
         <v>0</v>
@@ -32037,7 +32037,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="104">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G32" s="104">
         <v>0</v>
@@ -32063,7 +32063,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="104">
-        <v>0.33500000000000002</v>
+        <v>1</v>
       </c>
       <c r="G33" s="104">
         <v>1</v>
@@ -32083,7 +32083,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="104">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G34" s="104">
         <v>0</v>
@@ -32103,7 +32103,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="104">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G35" s="104">
         <v>0</v>
@@ -32129,7 +32129,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="104">
-        <v>0.33500000000000002</v>
+        <v>1</v>
       </c>
       <c r="G36" s="104">
         <v>1</v>
@@ -32149,7 +32149,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="104">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G37" s="104">
         <v>0</v>
@@ -32169,7 +32169,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="104">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G38" s="104">
         <v>0</v>
@@ -32195,7 +32195,7 @@
         <v>1</v>
       </c>
       <c r="F39" s="104">
-        <v>0.33500000000000002</v>
+        <v>1</v>
       </c>
       <c r="G39" s="104">
         <v>1</v>
@@ -32215,7 +32215,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="104">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G40" s="104">
         <v>0</v>
@@ -32235,7 +32235,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="104">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G41" s="104">
         <v>0</v>
@@ -32261,7 +32261,7 @@
         <v>0.3</v>
       </c>
       <c r="F42" s="104">
-        <v>0.33500000000000002</v>
+        <v>0.3</v>
       </c>
       <c r="G42" s="104">
         <v>0.3</v>
@@ -32281,7 +32281,7 @@
         <v>0.5</v>
       </c>
       <c r="F43" s="104">
-        <v>0.33500000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="G43" s="104">
         <v>0.5</v>
@@ -32301,7 +32301,7 @@
         <v>0.65</v>
       </c>
       <c r="F44" s="104">
-        <v>0.33500000000000002</v>
+        <v>0.65</v>
       </c>
       <c r="G44" s="104">
         <v>0.65</v>
@@ -32324,7 +32324,7 @@
         <v>0.3</v>
       </c>
       <c r="F45" s="104">
-        <v>0.33500000000000002</v>
+        <v>0.3</v>
       </c>
       <c r="G45" s="104">
         <v>0.3</v>
@@ -32344,7 +32344,7 @@
         <v>0.49</v>
       </c>
       <c r="F46" s="104">
-        <v>0.33500000000000002</v>
+        <v>0.49</v>
       </c>
       <c r="G46" s="104">
         <v>0.49</v>
@@ -32364,7 +32364,7 @@
         <v>0.52</v>
       </c>
       <c r="F47" s="104">
-        <v>0.33500000000000002</v>
+        <v>0.52</v>
       </c>
       <c r="G47" s="104">
         <v>0.52</v>
@@ -32390,7 +32390,7 @@
         <v>0.88</v>
       </c>
       <c r="F48" s="104">
-        <v>0.33500000000000002</v>
+        <v>0.88</v>
       </c>
       <c r="G48" s="104">
         <v>0.88</v>
@@ -32404,19 +32404,19 @@
         <v>262</v>
       </c>
       <c r="D49" s="104">
-        <v>0.93</v>
+        <v>0.78409090909090906</v>
       </c>
       <c r="E49" s="104">
-        <v>0.93</v>
+        <v>0.78409090909090906</v>
       </c>
       <c r="F49" s="104">
-        <v>0.33500000000000002</v>
+        <v>0.78409090909090906</v>
       </c>
       <c r="G49" s="104">
-        <v>0.93</v>
+        <v>0.78409090909090906</v>
       </c>
       <c r="H49" s="104">
-        <v>0.93</v>
+        <v>0.78409090909090906</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -32430,19 +32430,19 @@
         <v>261</v>
       </c>
       <c r="D50" s="104">
-        <v>1</v>
+        <v>0.88372093023255816</v>
       </c>
       <c r="E50" s="104">
-        <v>1</v>
+        <v>0.88372093023255816</v>
       </c>
       <c r="F50" s="104">
-        <v>0.33500000000000002</v>
+        <v>0.88372093023255816</v>
       </c>
       <c r="G50" s="104">
-        <v>1</v>
+        <v>0.88372093023255816</v>
       </c>
       <c r="H50" s="104">
-        <v>1</v>
+        <v>0.88372093023255816</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -32456,7 +32456,7 @@
         <v>0.86</v>
       </c>
       <c r="F51" s="104">
-        <v>0.33500000000000002</v>
+        <v>0.86</v>
       </c>
       <c r="G51" s="104">
         <v>0.86</v>
@@ -32482,7 +32482,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="F52" s="104">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G52" s="104">
         <v>0</v>
@@ -32502,7 +32502,7 @@
         <v>0.51</v>
       </c>
       <c r="F53" s="104">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G53" s="104">
         <v>0</v>
@@ -32564,15 +32564,15 @@
       </c>
       <c r="F57" s="104">
         <f t="shared" si="0"/>
-        <v>0.30150000000000005</v>
+        <v>0.35526315789473689</v>
       </c>
       <c r="G57" s="104">
         <f t="shared" si="0"/>
-        <v>0.30150000000000005</v>
+        <v>0.35526315789473689</v>
       </c>
       <c r="H57" s="104">
         <f t="shared" si="0"/>
-        <v>0.30150000000000005</v>
+        <v>0.35526315789473689</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -32589,15 +32589,15 @@
       </c>
       <c r="F58" s="104">
         <f t="shared" si="0"/>
-        <v>0.47820895522388057</v>
+        <v>0.27692307692307688</v>
       </c>
       <c r="G58" s="104">
         <f t="shared" si="0"/>
-        <v>0.47820895522388057</v>
+        <v>0.27692307692307688</v>
       </c>
       <c r="H58" s="104">
         <f t="shared" si="0"/>
-        <v>0.47820895522388057</v>
+        <v>0.27692307692307688</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -32997,7 +32997,7 @@
       </c>
       <c r="F73" s="104">
         <f t="shared" si="5"/>
-        <v>0.30150000000000005</v>
+        <v>0.63</v>
       </c>
       <c r="G73" s="104">
         <f t="shared" si="5"/>
@@ -33050,7 +33050,7 @@
       </c>
       <c r="F75" s="104">
         <f t="shared" si="7"/>
-        <v>0.30150000000000005</v>
+        <v>0.75600000000000001</v>
       </c>
       <c r="G75" s="104">
         <f t="shared" si="7"/>
@@ -33073,7 +33073,7 @@
       </c>
       <c r="D76" s="104">
         <f t="shared" ref="D76:H76" si="8">D21*0.9</f>
-        <v>0.63</v>
+        <v>0.2543478260869565</v>
       </c>
       <c r="E76" s="104">
         <f t="shared" si="8"/>
@@ -33081,7 +33081,7 @@
       </c>
       <c r="F76" s="104">
         <f t="shared" si="8"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G76" s="104">
         <f t="shared" si="8"/>
@@ -33106,7 +33106,7 @@
       </c>
       <c r="F77" s="104">
         <f t="shared" si="9"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G77" s="104">
         <f t="shared" si="9"/>
@@ -33129,7 +33129,7 @@
       </c>
       <c r="D78" s="104">
         <f t="shared" ref="D78:H78" si="10">D23*0.9</f>
-        <v>0.63</v>
+        <v>0.2543478260869565</v>
       </c>
       <c r="E78" s="104">
         <f t="shared" si="10"/>
@@ -33137,7 +33137,7 @@
       </c>
       <c r="F78" s="104">
         <f t="shared" si="10"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G78" s="104">
         <f t="shared" si="10"/>
@@ -33162,7 +33162,7 @@
       </c>
       <c r="F79" s="104">
         <f t="shared" si="11"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G79" s="104">
         <f t="shared" si="11"/>
@@ -33185,7 +33185,7 @@
       </c>
       <c r="D80" s="104">
         <f t="shared" ref="D80:H80" si="12">D25*0.9</f>
-        <v>0.63</v>
+        <v>0.2543478260869565</v>
       </c>
       <c r="E80" s="104">
         <f t="shared" si="12"/>
@@ -33193,7 +33193,7 @@
       </c>
       <c r="F80" s="104">
         <f t="shared" si="12"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G80" s="104">
         <f t="shared" si="12"/>
@@ -33218,7 +33218,7 @@
       </c>
       <c r="F81" s="104">
         <f t="shared" si="13"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G81" s="104">
         <f t="shared" si="13"/>
@@ -33249,7 +33249,7 @@
       </c>
       <c r="F82" s="104">
         <f t="shared" si="14"/>
-        <v>0.30150000000000005</v>
+        <v>0.9</v>
       </c>
       <c r="G82" s="104">
         <f t="shared" si="14"/>
@@ -33274,7 +33274,7 @@
       </c>
       <c r="F83" s="104">
         <f t="shared" si="15"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G83" s="104">
         <f t="shared" si="15"/>
@@ -33299,7 +33299,7 @@
       </c>
       <c r="F84" s="104">
         <f t="shared" si="16"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G84" s="104">
         <f t="shared" si="16"/>
@@ -33330,7 +33330,7 @@
       </c>
       <c r="F85" s="104">
         <f t="shared" si="17"/>
-        <v>0.30150000000000005</v>
+        <v>0.9</v>
       </c>
       <c r="G85" s="104">
         <f t="shared" si="17"/>
@@ -33355,7 +33355,7 @@
       </c>
       <c r="F86" s="104">
         <f t="shared" si="18"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G86" s="104">
         <f t="shared" si="18"/>
@@ -33380,7 +33380,7 @@
       </c>
       <c r="F87" s="104">
         <f t="shared" si="19"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G87" s="104">
         <f t="shared" si="19"/>
@@ -33411,7 +33411,7 @@
       </c>
       <c r="F88" s="104">
         <f t="shared" si="20"/>
-        <v>0.30150000000000005</v>
+        <v>0.9</v>
       </c>
       <c r="G88" s="104">
         <f t="shared" si="20"/>
@@ -33436,7 +33436,7 @@
       </c>
       <c r="F89" s="104">
         <f t="shared" si="21"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G89" s="104">
         <f t="shared" si="21"/>
@@ -33461,7 +33461,7 @@
       </c>
       <c r="F90" s="104">
         <f t="shared" si="22"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G90" s="104">
         <f t="shared" si="22"/>
@@ -33492,7 +33492,7 @@
       </c>
       <c r="F91" s="104">
         <f t="shared" si="23"/>
-        <v>0.30150000000000005</v>
+        <v>0.9</v>
       </c>
       <c r="G91" s="104">
         <f t="shared" si="23"/>
@@ -33517,7 +33517,7 @@
       </c>
       <c r="F92" s="104">
         <f t="shared" si="24"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G92" s="104">
         <f t="shared" si="24"/>
@@ -33542,7 +33542,7 @@
       </c>
       <c r="F93" s="104">
         <f t="shared" si="25"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G93" s="104">
         <f t="shared" si="25"/>
@@ -33573,7 +33573,7 @@
       </c>
       <c r="F94" s="104">
         <f t="shared" si="26"/>
-        <v>0.30150000000000005</v>
+        <v>0.9</v>
       </c>
       <c r="G94" s="104">
         <f t="shared" si="26"/>
@@ -33598,7 +33598,7 @@
       </c>
       <c r="F95" s="104">
         <f t="shared" si="27"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G95" s="104">
         <f t="shared" si="27"/>
@@ -33623,7 +33623,7 @@
       </c>
       <c r="F96" s="104">
         <f t="shared" si="28"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G96" s="104">
         <f t="shared" si="28"/>
@@ -33654,7 +33654,7 @@
       </c>
       <c r="F97" s="104">
         <f t="shared" si="29"/>
-        <v>0.30150000000000005</v>
+        <v>0.27</v>
       </c>
       <c r="G97" s="104">
         <f t="shared" si="29"/>
@@ -33679,7 +33679,7 @@
       </c>
       <c r="F98" s="104">
         <f t="shared" si="30"/>
-        <v>0.30150000000000005</v>
+        <v>0.45</v>
       </c>
       <c r="G98" s="104">
         <f t="shared" si="30"/>
@@ -33704,7 +33704,7 @@
       </c>
       <c r="F99" s="104">
         <f t="shared" si="31"/>
-        <v>0.30150000000000005</v>
+        <v>0.58500000000000008</v>
       </c>
       <c r="G99" s="104">
         <f t="shared" si="31"/>
@@ -33732,7 +33732,7 @@
       </c>
       <c r="F100" s="104">
         <f t="shared" si="32"/>
-        <v>0.30150000000000005</v>
+        <v>0.27</v>
       </c>
       <c r="G100" s="104">
         <f t="shared" si="32"/>
@@ -33757,7 +33757,7 @@
       </c>
       <c r="F101" s="104">
         <f t="shared" si="33"/>
-        <v>0.30150000000000005</v>
+        <v>0.441</v>
       </c>
       <c r="G101" s="104">
         <f t="shared" si="33"/>
@@ -33782,7 +33782,7 @@
       </c>
       <c r="F102" s="104">
         <f t="shared" si="34"/>
-        <v>0.30150000000000005</v>
+        <v>0.46800000000000003</v>
       </c>
       <c r="G102" s="104">
         <f t="shared" si="34"/>
@@ -33813,7 +33813,7 @@
       </c>
       <c r="F103" s="104">
         <f t="shared" si="35"/>
-        <v>0.30150000000000005</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="G103" s="104">
         <f t="shared" si="35"/>
@@ -33830,23 +33830,23 @@
       </c>
       <c r="D104" s="104">
         <f t="shared" ref="D104:H104" si="36">D49*0.9</f>
-        <v>0.83700000000000008</v>
+        <v>0.70568181818181819</v>
       </c>
       <c r="E104" s="104">
         <f t="shared" si="36"/>
-        <v>0.83700000000000008</v>
+        <v>0.70568181818181819</v>
       </c>
       <c r="F104" s="104">
         <f t="shared" si="36"/>
-        <v>0.30150000000000005</v>
+        <v>0.70568181818181819</v>
       </c>
       <c r="G104" s="104">
         <f t="shared" si="36"/>
-        <v>0.83700000000000008</v>
+        <v>0.70568181818181819</v>
       </c>
       <c r="H104" s="104">
         <f t="shared" si="36"/>
-        <v>0.83700000000000008</v>
+        <v>0.70568181818181819</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -33861,23 +33861,23 @@
       </c>
       <c r="D105" s="104">
         <f t="shared" ref="D105:H105" si="37">D50*0.9</f>
-        <v>0.9</v>
+        <v>0.79534883720930238</v>
       </c>
       <c r="E105" s="104">
         <f t="shared" si="37"/>
-        <v>0.9</v>
+        <v>0.79534883720930238</v>
       </c>
       <c r="F105" s="104">
         <f t="shared" si="37"/>
-        <v>0.30150000000000005</v>
+        <v>0.79534883720930238</v>
       </c>
       <c r="G105" s="104">
         <f t="shared" si="37"/>
-        <v>0.9</v>
+        <v>0.79534883720930238</v>
       </c>
       <c r="H105" s="104">
         <f t="shared" si="37"/>
-        <v>0.9</v>
+        <v>0.79534883720930238</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -33894,7 +33894,7 @@
       </c>
       <c r="F106" s="104">
         <f t="shared" si="38"/>
-        <v>0.30150000000000005</v>
+        <v>0.77400000000000002</v>
       </c>
       <c r="G106" s="104">
         <f t="shared" si="38"/>
@@ -33925,7 +33925,7 @@
       </c>
       <c r="F107" s="104">
         <f t="shared" si="39"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G107" s="104">
         <f t="shared" si="39"/>
@@ -33950,7 +33950,7 @@
       </c>
       <c r="F108" s="104">
         <f t="shared" si="40"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G108" s="104">
         <f t="shared" si="40"/>
@@ -34014,15 +34014,15 @@
       </c>
       <c r="F112" s="104">
         <f t="shared" si="41"/>
-        <v>0.35175000000000006</v>
+        <v>0.41447368421052638</v>
       </c>
       <c r="G112" s="104">
         <f t="shared" si="41"/>
-        <v>0.35175000000000006</v>
+        <v>0.41447368421052638</v>
       </c>
       <c r="H112" s="104">
         <f t="shared" si="41"/>
-        <v>0.35175000000000006</v>
+        <v>0.41447368421052638</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -34039,15 +34039,15 @@
       </c>
       <c r="F113" s="104">
         <f t="shared" si="41"/>
-        <v>0.55791044776119403</v>
+        <v>0.32307692307692304</v>
       </c>
       <c r="G113" s="104">
         <f t="shared" si="41"/>
-        <v>0.55791044776119403</v>
+        <v>0.32307692307692304</v>
       </c>
       <c r="H113" s="104">
         <f t="shared" si="41"/>
-        <v>0.55791044776119403</v>
+        <v>0.32307692307692304</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -34447,7 +34447,7 @@
       </c>
       <c r="F128" s="104">
         <f t="shared" si="46"/>
-        <v>0.35175000000000006</v>
+        <v>0.73499999999999999</v>
       </c>
       <c r="G128" s="104">
         <f t="shared" si="46"/>
@@ -34500,7 +34500,7 @@
       </c>
       <c r="F130" s="104">
         <f t="shared" si="48"/>
-        <v>0.35175000000000006</v>
+        <v>0.88200000000000001</v>
       </c>
       <c r="G130" s="104">
         <f t="shared" si="48"/>
@@ -34523,7 +34523,7 @@
       </c>
       <c r="D131" s="104">
         <f t="shared" ref="D131:H131" si="49">D21*1.05</f>
-        <v>0.73499999999999999</v>
+        <v>0.29673913043478262</v>
       </c>
       <c r="E131" s="104">
         <f t="shared" si="49"/>
@@ -34531,7 +34531,7 @@
       </c>
       <c r="F131" s="104">
         <f t="shared" si="49"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G131" s="104">
         <f t="shared" si="49"/>
@@ -34556,7 +34556,7 @@
       </c>
       <c r="F132" s="104">
         <f t="shared" si="50"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G132" s="104">
         <f t="shared" si="50"/>
@@ -34579,7 +34579,7 @@
       </c>
       <c r="D133" s="104">
         <f t="shared" ref="D133:H133" si="51">D23*1.05</f>
-        <v>0.73499999999999999</v>
+        <v>0.29673913043478262</v>
       </c>
       <c r="E133" s="104">
         <f t="shared" si="51"/>
@@ -34587,7 +34587,7 @@
       </c>
       <c r="F133" s="104">
         <f t="shared" si="51"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G133" s="104">
         <f t="shared" si="51"/>
@@ -34612,7 +34612,7 @@
       </c>
       <c r="F134" s="104">
         <f t="shared" si="52"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G134" s="104">
         <f t="shared" si="52"/>
@@ -34635,7 +34635,7 @@
       </c>
       <c r="D135" s="104">
         <f t="shared" ref="D135:H135" si="53">D25*1.05</f>
-        <v>0.73499999999999999</v>
+        <v>0.29673913043478262</v>
       </c>
       <c r="E135" s="104">
         <f t="shared" si="53"/>
@@ -34643,7 +34643,7 @@
       </c>
       <c r="F135" s="104">
         <f t="shared" si="53"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G135" s="104">
         <f t="shared" si="53"/>
@@ -34668,7 +34668,7 @@
       </c>
       <c r="F136" s="104">
         <f t="shared" si="54"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G136" s="104">
         <f t="shared" si="54"/>
@@ -34699,7 +34699,7 @@
       </c>
       <c r="F137" s="104">
         <f t="shared" si="55"/>
-        <v>0.35175000000000006</v>
+        <v>1.05</v>
       </c>
       <c r="G137" s="104">
         <f t="shared" si="55"/>
@@ -34724,7 +34724,7 @@
       </c>
       <c r="F138" s="104">
         <f t="shared" si="56"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G138" s="104">
         <f t="shared" si="56"/>
@@ -34749,7 +34749,7 @@
       </c>
       <c r="F139" s="104">
         <f t="shared" si="57"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G139" s="104">
         <f t="shared" si="57"/>
@@ -34780,7 +34780,7 @@
       </c>
       <c r="F140" s="104">
         <f t="shared" si="58"/>
-        <v>0.35175000000000006</v>
+        <v>1.05</v>
       </c>
       <c r="G140" s="104">
         <f t="shared" si="58"/>
@@ -34805,7 +34805,7 @@
       </c>
       <c r="F141" s="104">
         <f t="shared" si="59"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G141" s="104">
         <f t="shared" si="59"/>
@@ -34830,7 +34830,7 @@
       </c>
       <c r="F142" s="104">
         <f t="shared" si="60"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G142" s="104">
         <f t="shared" si="60"/>
@@ -34861,7 +34861,7 @@
       </c>
       <c r="F143" s="104">
         <f t="shared" si="61"/>
-        <v>0.35175000000000006</v>
+        <v>1.05</v>
       </c>
       <c r="G143" s="104">
         <f t="shared" si="61"/>
@@ -34886,7 +34886,7 @@
       </c>
       <c r="F144" s="104">
         <f t="shared" si="62"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G144" s="104">
         <f t="shared" si="62"/>
@@ -34911,7 +34911,7 @@
       </c>
       <c r="F145" s="104">
         <f t="shared" si="63"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G145" s="104">
         <f t="shared" si="63"/>
@@ -34942,7 +34942,7 @@
       </c>
       <c r="F146" s="104">
         <f t="shared" si="64"/>
-        <v>0.35175000000000006</v>
+        <v>1.05</v>
       </c>
       <c r="G146" s="104">
         <f t="shared" si="64"/>
@@ -34967,7 +34967,7 @@
       </c>
       <c r="F147" s="104">
         <f t="shared" si="65"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G147" s="104">
         <f t="shared" si="65"/>
@@ -34992,7 +34992,7 @@
       </c>
       <c r="F148" s="104">
         <f t="shared" si="66"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G148" s="104">
         <f t="shared" si="66"/>
@@ -35023,7 +35023,7 @@
       </c>
       <c r="F149" s="104">
         <f t="shared" si="67"/>
-        <v>0.35175000000000006</v>
+        <v>1.05</v>
       </c>
       <c r="G149" s="104">
         <f t="shared" si="67"/>
@@ -35048,7 +35048,7 @@
       </c>
       <c r="F150" s="104">
         <f t="shared" si="68"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G150" s="104">
         <f t="shared" si="68"/>
@@ -35073,7 +35073,7 @@
       </c>
       <c r="F151" s="104">
         <f t="shared" si="69"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G151" s="104">
         <f t="shared" si="69"/>
@@ -35104,7 +35104,7 @@
       </c>
       <c r="F152" s="104">
         <f t="shared" si="70"/>
-        <v>0.35175000000000006</v>
+        <v>0.315</v>
       </c>
       <c r="G152" s="104">
         <f t="shared" si="70"/>
@@ -35129,7 +35129,7 @@
       </c>
       <c r="F153" s="104">
         <f t="shared" si="71"/>
-        <v>0.35175000000000006</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="G153" s="104">
         <f t="shared" si="71"/>
@@ -35154,7 +35154,7 @@
       </c>
       <c r="F154" s="104">
         <f t="shared" si="72"/>
-        <v>0.35175000000000006</v>
+        <v>0.68250000000000011</v>
       </c>
       <c r="G154" s="104">
         <f t="shared" si="72"/>
@@ -35182,7 +35182,7 @@
       </c>
       <c r="F155" s="104">
         <f t="shared" si="73"/>
-        <v>0.35175000000000006</v>
+        <v>0.315</v>
       </c>
       <c r="G155" s="104">
         <f t="shared" si="73"/>
@@ -35207,7 +35207,7 @@
       </c>
       <c r="F156" s="104">
         <f t="shared" si="74"/>
-        <v>0.35175000000000006</v>
+        <v>0.51449999999999996</v>
       </c>
       <c r="G156" s="104">
         <f t="shared" si="74"/>
@@ -35232,7 +35232,7 @@
       </c>
       <c r="F157" s="104">
         <f t="shared" si="75"/>
-        <v>0.35175000000000006</v>
+        <v>0.54600000000000004</v>
       </c>
       <c r="G157" s="104">
         <f t="shared" si="75"/>
@@ -35263,7 +35263,7 @@
       </c>
       <c r="F158" s="104">
         <f t="shared" si="76"/>
-        <v>0.35175000000000006</v>
+        <v>0.92400000000000004</v>
       </c>
       <c r="G158" s="104">
         <f t="shared" si="76"/>
@@ -35280,23 +35280,23 @@
       </c>
       <c r="D159" s="104">
         <f t="shared" ref="D159:H159" si="77">D49*1.05</f>
-        <v>0.97650000000000015</v>
+        <v>0.8232954545454545</v>
       </c>
       <c r="E159" s="104">
         <f t="shared" si="77"/>
-        <v>0.97650000000000015</v>
+        <v>0.8232954545454545</v>
       </c>
       <c r="F159" s="104">
         <f t="shared" si="77"/>
-        <v>0.35175000000000006</v>
+        <v>0.8232954545454545</v>
       </c>
       <c r="G159" s="104">
         <f t="shared" si="77"/>
-        <v>0.97650000000000015</v>
+        <v>0.8232954545454545</v>
       </c>
       <c r="H159" s="104">
         <f t="shared" si="77"/>
-        <v>0.97650000000000015</v>
+        <v>0.8232954545454545</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -35311,23 +35311,23 @@
       </c>
       <c r="D160" s="104">
         <f t="shared" ref="D160:H160" si="78">D50*1.05</f>
-        <v>1.05</v>
+        <v>0.9279069767441861</v>
       </c>
       <c r="E160" s="104">
         <f t="shared" si="78"/>
-        <v>1.05</v>
+        <v>0.9279069767441861</v>
       </c>
       <c r="F160" s="104">
         <f t="shared" si="78"/>
-        <v>0.35175000000000006</v>
+        <v>0.9279069767441861</v>
       </c>
       <c r="G160" s="104">
         <f t="shared" si="78"/>
-        <v>1.05</v>
+        <v>0.9279069767441861</v>
       </c>
       <c r="H160" s="104">
         <f t="shared" si="78"/>
-        <v>1.05</v>
+        <v>0.9279069767441861</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
@@ -35344,7 +35344,7 @@
       </c>
       <c r="F161" s="104">
         <f t="shared" si="79"/>
-        <v>0.35175000000000006</v>
+        <v>0.90300000000000002</v>
       </c>
       <c r="G161" s="104">
         <f t="shared" si="79"/>
@@ -35375,7 +35375,7 @@
       </c>
       <c r="F162" s="104">
         <f t="shared" si="80"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G162" s="104">
         <f t="shared" si="80"/>
@@ -35400,7 +35400,7 @@
       </c>
       <c r="F163" s="104">
         <f t="shared" si="81"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G163" s="104">
         <f t="shared" si="81"/>
@@ -36997,15 +36997,15 @@
       <c r="B2" s="45" t="s">
         <v>138</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="115"/>
+      <c r="I2" s="115"/>
+      <c r="J2" s="115"/>
+      <c r="K2" s="115"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="45"/>
@@ -37017,15 +37017,15 @@
       <c r="B4" s="45" t="s">
         <v>138</v>
       </c>
-      <c r="C4" s="116"/>
-      <c r="D4" s="116"/>
-      <c r="E4" s="116"/>
-      <c r="F4" s="116"/>
-      <c r="G4" s="116"/>
-      <c r="H4" s="116"/>
-      <c r="I4" s="116"/>
-      <c r="J4" s="116"/>
-      <c r="K4" s="116"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
+      <c r="F4" s="115"/>
+      <c r="G4" s="115"/>
+      <c r="H4" s="115"/>
+      <c r="I4" s="115"/>
+      <c r="J4" s="115"/>
+      <c r="K4" s="115"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="45"/>
@@ -37037,43 +37037,43 @@
       <c r="B6" s="45" t="s">
         <v>138</v>
       </c>
-      <c r="C6" s="116"/>
-      <c r="D6" s="116"/>
-      <c r="E6" s="116"/>
-      <c r="F6" s="116"/>
-      <c r="G6" s="116"/>
-      <c r="H6" s="116"/>
-      <c r="I6" s="116"/>
-      <c r="J6" s="116"/>
-      <c r="K6" s="116"/>
+      <c r="C6" s="115"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="115"/>
+      <c r="H6" s="115"/>
+      <c r="I6" s="115"/>
+      <c r="J6" s="115"/>
+      <c r="K6" s="115"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="116"/>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="116"/>
-      <c r="G7" s="116"/>
-      <c r="H7" s="116"/>
-      <c r="I7" s="116"/>
-      <c r="J7" s="116"/>
-      <c r="K7" s="116"/>
+      <c r="C7" s="115"/>
+      <c r="D7" s="115"/>
+      <c r="E7" s="115"/>
+      <c r="F7" s="115"/>
+      <c r="G7" s="115"/>
+      <c r="H7" s="115"/>
+      <c r="I7" s="115"/>
+      <c r="J7" s="115"/>
+      <c r="K7" s="115"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="C8" s="116"/>
-      <c r="D8" s="116"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="116"/>
-      <c r="G8" s="116"/>
-      <c r="H8" s="116"/>
-      <c r="I8" s="116"/>
-      <c r="J8" s="116"/>
-      <c r="K8" s="116"/>
+      <c r="C8" s="115"/>
+      <c r="D8" s="115"/>
+      <c r="E8" s="115"/>
+      <c r="F8" s="115"/>
+      <c r="G8" s="115"/>
+      <c r="H8" s="115"/>
+      <c r="I8" s="115"/>
+      <c r="J8" s="115"/>
+      <c r="K8" s="115"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
@@ -37082,29 +37082,29 @@
       <c r="B10" s="45" t="s">
         <v>142</v>
       </c>
-      <c r="C10" s="116"/>
-      <c r="D10" s="116"/>
-      <c r="E10" s="116"/>
-      <c r="F10" s="116"/>
-      <c r="G10" s="116"/>
-      <c r="H10" s="116"/>
-      <c r="I10" s="116"/>
-      <c r="J10" s="116"/>
-      <c r="K10" s="116"/>
+      <c r="C10" s="115"/>
+      <c r="D10" s="115"/>
+      <c r="E10" s="115"/>
+      <c r="F10" s="115"/>
+      <c r="G10" s="115"/>
+      <c r="H10" s="115"/>
+      <c r="I10" s="115"/>
+      <c r="J10" s="115"/>
+      <c r="K10" s="115"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="45" t="s">
         <v>141</v>
       </c>
-      <c r="C11" s="116"/>
-      <c r="D11" s="116"/>
-      <c r="E11" s="116"/>
-      <c r="F11" s="116"/>
-      <c r="G11" s="116"/>
-      <c r="H11" s="116"/>
-      <c r="I11" s="116"/>
-      <c r="J11" s="116"/>
-      <c r="K11" s="116"/>
+      <c r="C11" s="115"/>
+      <c r="D11" s="115"/>
+      <c r="E11" s="115"/>
+      <c r="F11" s="115"/>
+      <c r="G11" s="115"/>
+      <c r="H11" s="115"/>
+      <c r="I11" s="115"/>
+      <c r="J11" s="115"/>
+      <c r="K11" s="115"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
@@ -37113,29 +37113,29 @@
       <c r="B13" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="C13" s="116"/>
-      <c r="D13" s="116"/>
-      <c r="E13" s="116"/>
-      <c r="F13" s="116"/>
-      <c r="G13" s="116"/>
-      <c r="H13" s="116"/>
-      <c r="I13" s="116"/>
-      <c r="J13" s="116"/>
-      <c r="K13" s="116"/>
+      <c r="C13" s="115"/>
+      <c r="D13" s="115"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="115"/>
+      <c r="H13" s="115"/>
+      <c r="I13" s="115"/>
+      <c r="J13" s="115"/>
+      <c r="K13" s="115"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="C14" s="116"/>
-      <c r="D14" s="116"/>
-      <c r="E14" s="116"/>
-      <c r="F14" s="116"/>
-      <c r="G14" s="116"/>
-      <c r="H14" s="116"/>
-      <c r="I14" s="116"/>
-      <c r="J14" s="116"/>
-      <c r="K14" s="116"/>
+      <c r="C14" s="115"/>
+      <c r="D14" s="115"/>
+      <c r="E14" s="115"/>
+      <c r="F14" s="115"/>
+      <c r="G14" s="115"/>
+      <c r="H14" s="115"/>
+      <c r="I14" s="115"/>
+      <c r="J14" s="115"/>
+      <c r="K14" s="115"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="RgdAR3BFtcGQtrRbSdQKBGo+vA8vXft2CfMoIPNylw2Kgtq5Y60OF/gu0FwTwlYUkXD70DqSCseNkguXFqARBA==" saltValue="Mz7gePsAVXfIyQ62rOG4NQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
@@ -37174,7 +37174,7 @@
       <c r="A2" s="27" t="s">
         <v>330</v>
       </c>
-      <c r="B2" s="117">
+      <c r="B2" s="116">
         <v>10</v>
       </c>
     </row>
@@ -37182,7 +37182,7 @@
       <c r="A3" s="27" t="s">
         <v>331</v>
       </c>
-      <c r="B3" s="117">
+      <c r="B3" s="116">
         <v>10</v>
       </c>
     </row>
@@ -37190,7 +37190,7 @@
       <c r="A4" s="27" t="s">
         <v>325</v>
       </c>
-      <c r="B4" s="117">
+      <c r="B4" s="116">
         <v>50</v>
       </c>
     </row>
@@ -37198,7 +37198,7 @@
       <c r="A5" s="27" t="s">
         <v>329</v>
       </c>
-      <c r="B5" s="117">
+      <c r="B5" s="116">
         <v>100</v>
       </c>
     </row>
@@ -37206,7 +37206,7 @@
       <c r="A6" s="27" t="s">
         <v>332</v>
       </c>
-      <c r="B6" s="117">
+      <c r="B6" s="116">
         <v>5</v>
       </c>
     </row>
@@ -37214,7 +37214,7 @@
       <c r="A7" s="27" t="s">
         <v>333</v>
       </c>
-      <c r="B7" s="117">
+      <c r="B7" s="116">
         <v>5</v>
       </c>
     </row>

</xml_diff>